<commit_message>
added 160 tweeter text
</commit_message>
<xml_diff>
--- a/Social Media.xlsx
+++ b/Social Media.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="331">
   <si>
     <t>nyithidho adhola wityeko ye winjo athem mawan manyen</t>
   </si>
@@ -529,13 +529,493 @@
   </si>
   <si>
     <t>Iwondo wan</t>
+  </si>
+  <si>
+    <t>Ŋat mar-aryo otho #COVID19 i Uganda: dhako ma jaöro 80 mawuok Mengo, Kisenyi III, Kampala.</t>
+  </si>
+  <si>
+    <t>Ŋa mafuodi cayo?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lwok cingi gi sabun kod pii macuer, kis hongo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boy umi kod dhoki gi MASK ka intie i dier ji </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cam ciemo makonyi limo cir </t>
+  </si>
+  <si>
+    <t>Ikir'igeey waŋi kosa umi kosa dhoki gi cingi ma k'olony.</t>
+  </si>
+  <si>
+    <t>Wey fut 5 ama i dier in kod ŋat man</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To poy kurrok maber. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bed gi wikend m'okwe. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Korona Ki Tuodo </t>
+  </si>
+  <si>
+    <t>Paka candi m'obino gi COVID-19 nyalo rwako tic i Afrika</t>
+  </si>
+  <si>
+    <t>Gin aŋo ma timere Tororo?</t>
+  </si>
+  <si>
+    <t>Onyango osekwo/osekuo kuom tuo mar ich kach.</t>
+  </si>
+  <si>
+    <t>ja-Luo acyel oringa</t>
+  </si>
+  <si>
+    <t>Kwo cakere kama luoro gik iye</t>
+  </si>
+  <si>
+    <t>Paka wamedere gi ruko with medical mask i dier jo man a paka wadiyo ye nyay ma COVID.</t>
+  </si>
+  <si>
+    <t>Wac pa ŋat moro: "Ma kicutho, cimere gi limo dongo ma aperi kwoŋ aperin."</t>
+  </si>
+  <si>
+    <t>Ka itieko cungo m'otire, t'ineno ye jothu'in ma inyalo konyo. Karago, ipenjere ni to kwoŋ jo me ŋa won mamito dongo, aka ŋa mere ma lacuto woko acuta pesa nin.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T'imiyo kony ri jo no kende ma jodwaro dongrok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Awinjo meno. </t>
+  </si>
+  <si>
+    <t>Indir madit wakonyo ji kada manyap rupir walworo junywol pajo kosa walworo awacha mapiny.</t>
+  </si>
+  <si>
+    <t>Yoo ma ikiluor a ma ogwaŋ mako in iye</t>
+  </si>
+  <si>
+    <t>Maa akia kata uwacho nadi?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liverpool oloyo i English Premier League ma oro 2019/20. </t>
+  </si>
+  <si>
+    <t>Otero jo oro 30 limo ye telo i tuko me.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ji ciegin romo 700 ka. Ber. </t>
+  </si>
+  <si>
+    <t>Ka poyo nitie gima ber awira, mondo an ofwoy limo ryeko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Namba iidhó maber </t>
+  </si>
+  <si>
+    <t>ru megi gik ye cien adec, to ki wác.</t>
+  </si>
+  <si>
+    <t>Ng'at ma ineno i wi got k'opodho koro apodha.</t>
+  </si>
+  <si>
+    <t>Yie nimo ka chiegni gowo</t>
+  </si>
+  <si>
+    <t>Pii fuonjo wa ni ka wapye, wabedo maler.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kendó nyaŋith ka opye nyalo wodho paro ma di ryeko, paka Isaac Newton ma oniaŋ kwoŋ "Gravity" kareno go obedo ri go abeda moth i tyend yath olemo.</t>
+  </si>
+  <si>
+    <t>Kwoŋ kis apar ma kwó perin, acyel mere bedo gima timere kwoŋ in, aka aboŋwen mere bedo kit ma itiiyere kod gima timere kwoŋ in.</t>
+  </si>
+  <si>
+    <t>Kitawin konyo nyutho dhano ni paro pere ma ciene no ki nyien tektek</t>
+  </si>
+  <si>
+    <t>Wuok ka 31, May,  @MinofHealthUG ocako tuco</t>
+  </si>
+  <si>
+    <t>Ri ameno, kada nende lockdown oluogere ma onyo omiyo ji thuolo moro, wapoy bende ni "kwo oloyo ŋaŋo."</t>
+  </si>
+  <si>
+    <t>Wakinyal romo dhano winjo wac ma go k'oyikere jolo, to kada dicyel wakir-wacay men ma nitie i piidho kodhi</t>
+  </si>
+  <si>
+    <t>Wawe' gi kenyo…</t>
+  </si>
+  <si>
+    <t>Onyay loka Kenya, jowuotan!</t>
+  </si>
+  <si>
+    <t>Wageng Korona</t>
+  </si>
+  <si>
+    <t>Ru megi, won ot goyo rangi i kor ot m'oti, ma wuondo jo ni fuodi nyien.</t>
+  </si>
+  <si>
+    <t>Agulu pii tho i dho-gola</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A m'omiyo ka imito nywomo kosa nywomrok, ikir'iyeere nyaka gi cal acala pa dhano.</t>
+  </si>
+  <si>
+    <t>Kwo ka kilokere mayot, in medere bedo ma itek ayin.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nen maloyo ŋono kosa pesa. </t>
+  </si>
+  <si>
+    <t>Yaw iye inen maber.</t>
+  </si>
+  <si>
+    <t>Piny tek</t>
+  </si>
+  <si>
+    <t>In bende</t>
+  </si>
+  <si>
+    <t>I kwo, ini gi yero kwoŋ aryo:lokere jacako gir-atima, kosa tiiy ri go.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ikiŋeey kama jawuodhi' ma imaro owuok iye. </t>
+  </si>
+  <si>
+    <t>Doŋ gi boor.</t>
+  </si>
+  <si>
+    <t>Ikuya ni ŋa won ma iroomo gine.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bed gi booR ma iweyo mita 4 ama i dier in kod dhano man sawa jye. </t>
+  </si>
+  <si>
+    <t>Bedo boor boor gi ji a acyel kwoŋ gima ber ítimo ka ila nyalo geŋo COVID-19.</t>
+  </si>
+  <si>
+    <t>Bero ma imiyo ŋat man winjo, waco mathoth kwoŋ in.</t>
+  </si>
+  <si>
+    <t>Fuonjo nyaŋith peri' ma ikifuonjo cunyi' meno ki fuonjrok kada acyel.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ber an gi penjo. </t>
+  </si>
+  <si>
+    <t>Juogi nitie Par'Adhola?</t>
+  </si>
+  <si>
+    <t>Imito timo gin aŋo gi juogi?</t>
+  </si>
+  <si>
+    <t>Tic gi jotur cik ma piny omiyo.</t>
+  </si>
+  <si>
+    <t>La tundo ka 5 i dwee mar abic ma wadonjo iye ni.</t>
+  </si>
+  <si>
+    <t>Wan i Uganda korni watemo geŋo twoo Korona ka wabedo peco  tieko ndelo makalo 45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yido asoma nen Kwon perin makononi </t>
+  </si>
+  <si>
+    <t>Nen kwo peri' ma konon imiy duoŋ.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Okadho! Ikir'iture ri gima yowaŋe; fuodi k'otundo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ikir'iywak gim'okadho. </t>
+  </si>
+  <si>
+    <t>Ka iwacho i Dholuo-Kenya ni "dhow ni tek manade ni," iloko i Dhopadhola ni "dhodhok ni tek manedi ni"</t>
+  </si>
+  <si>
+    <t>Dhyaŋ kiwey madho pi i jwom ru ogwal maywak dho ume</t>
+  </si>
+  <si>
+    <t>A cow doesn't stop drinking water from the well because of a croaking frog next to its nostrils</t>
+  </si>
+  <si>
+    <t>Kwoη kis apar ma kwó perin, acyel mere bedo gima timere kwoη in aka aboηwen mere bedo kit ma itiiyere kod gima timere kwoη in.</t>
+  </si>
+  <si>
+    <t>Minista Ruth Aceng' kwayo mon Uganda ni mondo j'owere gi jogueco lor.</t>
+  </si>
+  <si>
+    <t>Kwó ki lokere mayot; medere bedo ma itek ayin.</t>
+  </si>
+  <si>
+    <t>Ng'ato calo janeko ye.</t>
+  </si>
+  <si>
+    <t>Dhano ma wiye otire goyo nedi adha mere?</t>
+  </si>
+  <si>
+    <t>Wapenj jo madongo.</t>
+  </si>
+  <si>
+    <t>Ng'a mapiemo gi Kaguta Museveni ?</t>
+  </si>
+  <si>
+    <t>Ere ba! Bonyo omuonjo Uganda kendo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Waη ni i thotho maloyo m'okadho ca.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> #OVID19 gi ka, bonyo gi kaca. </t>
+  </si>
+  <si>
+    <t>Rupiny!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ka wawodho ndiiko i Dhopadhola, bedo gimaber ka owuok ma ondikere maber kendo ma somere gi yoto. </t>
+  </si>
+  <si>
+    <t>To ndiiko ma cal pa jamwa a m'ondiko kwoto kiri wii jo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nitie gima owuok ma makere gi COVID19 ma calo oido ber obed Dhopadhola, to ka ineno!</t>
+  </si>
+  <si>
+    <t>Wer mamit ba!</t>
+  </si>
+  <si>
+    <t>To, Acoli keken?</t>
+  </si>
+  <si>
+    <t>Lwok cingi' tektek gi sabun.</t>
+  </si>
+  <si>
+    <t>Nyay wac wanyal geηo</t>
+  </si>
+  <si>
+    <t>Ka inen iduoko wok DUBAI, UAE kosa iηeeyo ηat moro m'owok koro i dwe mar-adek (March) me mondo lwoη jo-Ministry Of Health ka igoyo ri jo simo ama:</t>
+  </si>
+  <si>
+    <t>Wan jo jye ber wabed ma kis dhano dewo kwoη ηat man, to wariwere ka wakonyere gwoko piny mawan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COVID19 obedo lweny, ma wanyalo loyo nyaka ka wariwo cing-wan kanyacyel paka jo-Uganda. </t>
+  </si>
+  <si>
+    <t>Kuya lyec bano wuoth pere nedi ka dok m'omer !</t>
+  </si>
+  <si>
+    <t>Wakinyal romo dhano winjo wac ma go k'oyikere jolo, to kada di-cyel wakir-wacay men ma nitie i piídho kodhi</t>
+  </si>
+  <si>
+    <t>Wakony jo mawan kuro lonyo ma wacowere.</t>
+  </si>
+  <si>
+    <t>Kada wakimít nyero nago</t>
+  </si>
+  <si>
+    <t>Kis nyathi mbiji acyel</t>
+  </si>
+  <si>
+    <t>Ri ji acyel acyele.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wac me pooyo nyalo bero. </t>
+  </si>
+  <si>
+    <t>Aka pooy ni jo-Iran jo-Islam</t>
+  </si>
+  <si>
+    <t>Kenyo jajera waco, "thu gi silwany!"</t>
+  </si>
+  <si>
+    <t>Ini gi jokwor?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Meno ber.</t>
+  </si>
+  <si>
+    <t>Nyutho ni icungo ri gimoro, gimoro i kwo perin</t>
+  </si>
+  <si>
+    <t>pa-winj wac me</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jo ma kano pesa pa jo akana i bank joηaηο bank. </t>
+  </si>
+  <si>
+    <t>Jo ma ni gi anywola-lim moro jomiyere ηaηο.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pesa obedo kodhi. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kodhi no ki kony ka bedo abeda i dhokin kosa i bank. </t>
+  </si>
+  <si>
+    <t>Piidh kodhi i lowo (gir-atima), ikeeci acama</t>
+  </si>
+  <si>
+    <t>Those who save in banks are making the bank rich.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Those who have investments are making themselves rich.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Money is a seed. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seeds serve no purpose being in your mouth or in the bank. </t>
+  </si>
+  <si>
+    <t>Plant your seeds in the ground (investments), and eat your harvest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Konon obedo International Mother Language Day. </t>
+  </si>
+  <si>
+    <t>COM WANG'IN</t>
+  </si>
+  <si>
+    <t>Ka imito nwaηο gino tektek, ila ripo ketho miyrok, t'icomo waηin iye, t'irwako cunyin iye.</t>
+  </si>
+  <si>
+    <t>Bed gi weekend m'okwe, gi siem kende kende.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ja-Luo nywomo nyar Kabaka</t>
+  </si>
+  <si>
+    <t>Apenjo: dhano kwalo nedi mo i transfoma ma alektwist  luw'iye?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ka inen go okidhο kareno sitima nitie "off," onyalo ridho nedi ni sitima kóduoki "on" i sawa wo' meno? </t>
+  </si>
+  <si>
+    <t>Ogonyo waya kutho?</t>
+  </si>
+  <si>
+    <t>Wamak tic gi men waget thu'wan.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jo mathoth jorendere tundo kama wi gin wiil kodi kit gin mar-adieri, aka j'orwenyo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kwo mar-adieri miyi' yoto loyo kwó ma tuod</t>
+  </si>
+  <si>
+    <t>Ng'a m'owaco ni ber iwuoth kosa iluuw pa jadwoη moro?</t>
+  </si>
+  <si>
+    <t>Ikir'irendere ni iηaη</t>
+  </si>
+  <si>
+    <t>Medrok ang'o?</t>
+  </si>
+  <si>
+    <t>Paka niaη peri' medere a paka ikidho ka inok gi tim ma sisiri kodi tim ma nyageerogeero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meno ber. </t>
+  </si>
+  <si>
+    <t>Nyutho ni icungo ri gimoro, gimoro i kwó perin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ini gi jokwor? </t>
+  </si>
+  <si>
+    <t>Aloko cal.</t>
+  </si>
+  <si>
+    <t>Gin cha nyay.</t>
+  </si>
+  <si>
+    <t>Fuonjo nyaηith perin ma ikifuonjo cunyin meno ki fuonjrok kada acyel.</t>
+  </si>
+  <si>
+    <t>Gwokrok kuoη "Wuhan coronavirus"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ongo' gima la tic. </t>
+  </si>
+  <si>
+    <t>In ayin.</t>
+  </si>
+  <si>
+    <t>Gavment oketho wac ni dhano okan ciemo, piri wac bino wuok Kenya nike bonyo laro yo-Uganda.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bonyo ciegin donjo Uganda, wuok Kenya. </t>
+  </si>
+  <si>
+    <t>Yìkere.</t>
+  </si>
+  <si>
+    <t>Jago ma UK,  @BorisJohnson , ociko paka UK la tiiyere gi Afrika, nike Afrika ni gi cungo maber, aka cungo me kidho dongo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Onyutho ama i cokrok pere London gi jotel Africa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nike riiηο dhyaη wuok Uganda la limo katale i UK. </t>
+  </si>
+  <si>
+    <t>Wacak kune?</t>
+  </si>
+  <si>
+    <t>Kwó cakere kama luoro gik iye"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ongo gima nono. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> i piny me, ka ineno jo mathoth, cal pa kis acyel dwaro apere. </t>
+  </si>
+  <si>
+    <t>Kiri jo madongo, aka me a teko.</t>
+  </si>
+  <si>
+    <t>Kole amumyiyo awacho ni ju timi tich ma volunteer ma oro achiel…</t>
+  </si>
+  <si>
+    <t>Uganda Industrial Research Institute oyawo ka-tiek ma tiche m'opokere opokere i Namanve Industrial Area.</t>
+  </si>
+  <si>
+    <t>Eno apa-winj wac me ka imaro juko kosa yeyo motoka moro jye, kada ma k'obedo PSV, ni otiηin.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mondo inyalo jwango kwó perin ri jonek!</t>
+  </si>
+  <si>
+    <t>Wakinyal romo dhano wiinjo wac ma go k'oyikere jolo to kada di-cyel,wair-wacay men ma nitie i</t>
+  </si>
+  <si>
+    <t>Dhier obedo Kayunga monyo Imam acyel ogik onwaηο ni ciege manyien obedo jacwo</t>
+  </si>
+  <si>
+    <t>Nike ni: 'Oido arango dhako anywoma.'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monyo apodho kwoη nyako maηon m'oruko hijab, akwayo go omitan to go yeyo. </t>
+  </si>
+  <si>
+    <t>Wabino wacako mare</t>
+  </si>
+  <si>
+    <t>Afwoyo jo m'oluwa' konon.</t>
+  </si>
+  <si>
+    <t>Ayenyo ye "followers" 1000, to ki rach kada achak gi 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -553,6 +1033,12 @@
       <sz val="10"/>
       <color rgb="FF1C1E21"/>
       <name val="Inherit"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF14171A"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -575,7 +1061,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -585,6 +1071,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,6 +1079,176 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1025" name="AutoShape 1" descr="White heavy check mark"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="3048000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1026" name="AutoShape 2" descr="White heavy check mark"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="3657600"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1027" name="AutoShape 3" descr="White heavy check mark"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="4267200"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1028" name="AutoShape 4" descr="White heavy check mark"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="4876800"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1029" name="AutoShape 5" descr="Negative squared cross mark"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="5486400"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1693,10 +2350,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:B12"/>
+  <dimension ref="A2:B166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="A146" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1762,8 +2419,798 @@
         <v>170</v>
       </c>
     </row>
+    <row r="13" spans="1:2" ht="30">
+      <c r="A13" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="16.5">
+      <c r="A17" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="16.5">
+      <c r="A18" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="16.5">
+      <c r="A20" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="16.5">
+      <c r="A21" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="16.5">
+      <c r="A22" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="16.5">
+      <c r="A23" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="16.5">
+      <c r="A24" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="16.5">
+      <c r="A25" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="16.5">
+      <c r="A26" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="16.5">
+      <c r="A27" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="16.5">
+      <c r="A28" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="16.5">
+      <c r="A29" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="16.5">
+      <c r="A30" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="16.5">
+      <c r="A31" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="16.5">
+      <c r="A33" s="5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="16.5">
+      <c r="A34" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="16.5">
+      <c r="A35" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="16.5">
+      <c r="A36" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="16.5">
+      <c r="A37" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="16.5">
+      <c r="A38" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="16.5">
+      <c r="A39" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="16.5">
+      <c r="A40" s="5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="16.5">
+      <c r="A41" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="16.5">
+      <c r="A42" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="16.5">
+      <c r="A43" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="16.5">
+      <c r="A44" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="16.5">
+      <c r="A45" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="16.5">
+      <c r="A46" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="16.5">
+      <c r="A47" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="16.5">
+      <c r="A48" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="16.5">
+      <c r="A50" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="16.5">
+      <c r="A51" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="16.5">
+      <c r="A52" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="16.5">
+      <c r="A53" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="16.5">
+      <c r="A54" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="16.5">
+      <c r="A55" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="16.5">
+      <c r="A56" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="16.5">
+      <c r="A57" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="16.5">
+      <c r="A58" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="16.5">
+      <c r="A59" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="16.5">
+      <c r="A60" s="5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="16.5">
+      <c r="A61" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" ht="30">
+      <c r="A63" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="16.5">
+      <c r="A64" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>238</v>
+      </c>
+      <c r="B80" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" ht="16.5">
+      <c r="A108" s="5" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
+        <v>275</v>
+      </c>
+      <c r="B116" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>276</v>
+      </c>
+      <c r="B117" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" t="s">
+        <v>277</v>
+      </c>
+      <c r="B118" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" t="s">
+        <v>278</v>
+      </c>
+      <c r="B119" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" t="s">
+        <v>279</v>
+      </c>
+      <c r="B120" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" ht="16.5">
+      <c r="A136" s="5" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" ht="16.5">
+      <c r="A145" s="5" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" ht="30">
+      <c r="A148" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" ht="16.5">
+      <c r="A153" s="5" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" ht="30">
+      <c r="A162" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1">
+      <c r="A165" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" t="s">
+        <v>330</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>